<commit_message>
updated some pseudo code editSystem
</commit_message>
<xml_diff>
--- a/Pseudo Code/editSystem.xlsx
+++ b/Pseudo Code/editSystem.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Pseudo Code</t>
   </si>
@@ -56,7 +56,31 @@
     <t>editSystem()</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>userName String</t>
+  </si>
+  <si>
+    <t>newUserName String</t>
+  </si>
+  <si>
+    <t>userName = newUserName</t>
+  </si>
+  <si>
+    <t>commit changes</t>
+  </si>
+  <si>
+    <t>\\admin able to edit users information</t>
+  </si>
+  <si>
+    <t>newEmail</t>
+  </si>
+  <si>
+    <t>email = newEmail</t>
+  </si>
+  <si>
+    <t>newName</t>
+  </si>
+  <si>
+    <t>name - newName</t>
   </si>
 </sst>
 </file>
@@ -410,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,17 +473,25 @@
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
@@ -500,31 +532,31 @@
       <c r="A16" s="3"/>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -532,37 +564,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="5" t="s">
         <v>8</v>

</xml_diff>